<commit_message>
push dev to main branch
</commit_message>
<xml_diff>
--- a/todolist_game_MVP.xlsx
+++ b/todolist_game_MVP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t xml:space="preserve">Rétroplanning jeu Clash of Zombie (version MVP)</t>
   </si>
@@ -154,10 +154,13 @@
     <t xml:space="preserve">Acces depuis Itch.io</t>
   </si>
   <si>
-    <t xml:space="preserve">plateforme Windows, MacOS, et linux</t>
+    <t xml:space="preserve">When downloaded, must run on Windows, MacOS, and linux, 32 and 64 bits ‘puters</t>
   </si>
   <si>
-    <t xml:space="preserve">PC 32 et 64 bites</t>
+    <t xml:space="preserve">Export Ressources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convert source code in Lua to Javascript for HTML support.</t>
   </si>
   <si>
     <t xml:space="preserve">Traduction en englais</t>
@@ -836,9 +839,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>124920</xdr:colOff>
+      <xdr:colOff>124560</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>321120</xdr:rowOff>
+      <xdr:rowOff>320760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -852,7 +855,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8897040" y="877680"/>
-          <a:ext cx="5757480" cy="4317840"/>
+          <a:ext cx="5757120" cy="4317480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1076,8 +1079,8 @@
   </sheetPr>
   <dimension ref="A1:AC1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B42" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2644,6 +2647,20 @@
       <c r="AC71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B72" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="28"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="26"/>
+      <c r="I72" s="27"/>
+      <c r="J72" s="26"/>
+      <c r="K72" s="27"/>
+      <c r="L72" s="26"/>
+      <c r="M72" s="27"/>
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
       <c r="Q72" s="2"/>
@@ -2661,6 +2678,22 @@
       <c r="AC72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B73" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C73" s="25"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F73" s="26"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="27"/>
+      <c r="J73" s="26"/>
+      <c r="K73" s="27"/>
+      <c r="L73" s="26"/>
+      <c r="M73" s="27"/>
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
       <c r="Q73" s="2"/>
@@ -2677,8 +2710,24 @@
       <c r="AB73" s="2"/>
       <c r="AC73" s="2"/>
     </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="2"/>
+      <c r="B74" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F74" s="26"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="27"/>
+      <c r="J74" s="26"/>
+      <c r="K74" s="27"/>
+      <c r="L74" s="26"/>
+      <c r="M74" s="27"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
@@ -2696,8 +2745,24 @@
       <c r="AB74" s="2"/>
       <c r="AC74" s="2"/>
     </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="26.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="2"/>
+      <c r="B75" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="25"/>
+      <c r="D75" s="25"/>
+      <c r="E75" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F75" s="26"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="26"/>
+      <c r="I75" s="27"/>
+      <c r="J75" s="26"/>
+      <c r="K75" s="27"/>
+      <c r="L75" s="26"/>
+      <c r="M75" s="27"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
@@ -2717,6 +2782,20 @@
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F76" s="26"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="26"/>
+      <c r="I76" s="27"/>
+      <c r="J76" s="26"/>
+      <c r="K76" s="27"/>
+      <c r="L76" s="26"/>
+      <c r="M76" s="27"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>
@@ -2736,6 +2815,20 @@
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F77" s="26"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="26"/>
+      <c r="I77" s="27"/>
+      <c r="J77" s="26"/>
+      <c r="K77" s="27"/>
+      <c r="L77" s="26"/>
+      <c r="M77" s="27"/>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
@@ -2755,6 +2848,20 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F78" s="26"/>
+      <c r="G78" s="27"/>
+      <c r="H78" s="26"/>
+      <c r="I78" s="27"/>
+      <c r="J78" s="26"/>
+      <c r="K78" s="27"/>
+      <c r="L78" s="26"/>
+      <c r="M78" s="27"/>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
@@ -2774,6 +2881,20 @@
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="2"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="26"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="26"/>
+      <c r="I79" s="27"/>
+      <c r="J79" s="26"/>
+      <c r="K79" s="27"/>
+      <c r="L79" s="26"/>
+      <c r="M79" s="27"/>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
@@ -2793,6 +2914,20 @@
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="2"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F80" s="26"/>
+      <c r="G80" s="27"/>
+      <c r="H80" s="26"/>
+      <c r="I80" s="27"/>
+      <c r="J80" s="26"/>
+      <c r="K80" s="27"/>
+      <c r="L80" s="26"/>
+      <c r="M80" s="27"/>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
@@ -2812,6 +2947,20 @@
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="2"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F81" s="26"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="26"/>
+      <c r="I81" s="27"/>
+      <c r="J81" s="26"/>
+      <c r="K81" s="27"/>
+      <c r="L81" s="26"/>
+      <c r="M81" s="27"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
@@ -2831,6 +2980,22 @@
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="2"/>
+      <c r="B82" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F82" s="26"/>
+      <c r="G82" s="27"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="27"/>
+      <c r="J82" s="26"/>
+      <c r="K82" s="27"/>
+      <c r="L82" s="26"/>
+      <c r="M82" s="27"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
       <c r="P82" s="2"/>
@@ -2850,6 +3015,20 @@
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="2"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F83" s="26"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="26"/>
+      <c r="I83" s="27"/>
+      <c r="J83" s="26"/>
+      <c r="K83" s="27"/>
+      <c r="L83" s="26"/>
+      <c r="M83" s="27"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
       <c r="P83" s="2"/>
@@ -2869,6 +3048,22 @@
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="2"/>
+      <c r="B84" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F84" s="30"/>
+      <c r="G84" s="31"/>
+      <c r="H84" s="30"/>
+      <c r="I84" s="31"/>
+      <c r="J84" s="30"/>
+      <c r="K84" s="31"/>
+      <c r="L84" s="30"/>
+      <c r="M84" s="31"/>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
       <c r="P84" s="2"/>
@@ -3140,20 +3335,18 @@
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="2"/>
-      <c r="B96" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="26"/>
-      <c r="G96" s="27"/>
-      <c r="H96" s="26"/>
-      <c r="I96" s="27"/>
-      <c r="J96" s="26"/>
-      <c r="K96" s="27"/>
-      <c r="L96" s="26"/>
-      <c r="M96" s="27"/>
+      <c r="B96" s="0"/>
+      <c r="C96" s="0"/>
+      <c r="D96" s="0"/>
+      <c r="E96" s="0"/>
+      <c r="F96" s="0"/>
+      <c r="G96" s="0"/>
+      <c r="H96" s="0"/>
+      <c r="I96" s="0"/>
+      <c r="J96" s="0"/>
+      <c r="K96" s="0"/>
+      <c r="L96" s="0"/>
+      <c r="M96" s="0"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
@@ -3173,22 +3366,18 @@
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2"/>
-      <c r="B97" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F97" s="26"/>
-      <c r="G97" s="27"/>
-      <c r="H97" s="26"/>
-      <c r="I97" s="27"/>
-      <c r="J97" s="26"/>
-      <c r="K97" s="27"/>
-      <c r="L97" s="26"/>
-      <c r="M97" s="27"/>
+      <c r="B97" s="0"/>
+      <c r="C97" s="0"/>
+      <c r="D97" s="0"/>
+      <c r="E97" s="0"/>
+      <c r="F97" s="0"/>
+      <c r="G97" s="0"/>
+      <c r="H97" s="0"/>
+      <c r="I97" s="0"/>
+      <c r="J97" s="0"/>
+      <c r="K97" s="0"/>
+      <c r="L97" s="0"/>
+      <c r="M97" s="0"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
       <c r="P97" s="2"/>
@@ -3208,22 +3397,18 @@
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2"/>
-      <c r="B98" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F98" s="26"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="26"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="26"/>
-      <c r="K98" s="27"/>
-      <c r="L98" s="26"/>
-      <c r="M98" s="27"/>
+      <c r="B98" s="0"/>
+      <c r="C98" s="0"/>
+      <c r="D98" s="0"/>
+      <c r="E98" s="0"/>
+      <c r="F98" s="0"/>
+      <c r="G98" s="0"/>
+      <c r="H98" s="0"/>
+      <c r="I98" s="0"/>
+      <c r="J98" s="0"/>
+      <c r="K98" s="0"/>
+      <c r="L98" s="0"/>
+      <c r="M98" s="0"/>
       <c r="N98" s="2"/>
       <c r="O98" s="2"/>
       <c r="P98" s="2"/>
@@ -3243,22 +3428,18 @@
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2"/>
-      <c r="B99" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F99" s="26"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="26"/>
-      <c r="I99" s="27"/>
-      <c r="J99" s="26"/>
-      <c r="K99" s="27"/>
-      <c r="L99" s="26"/>
-      <c r="M99" s="27"/>
+      <c r="B99" s="0"/>
+      <c r="C99" s="0"/>
+      <c r="D99" s="0"/>
+      <c r="E99" s="0"/>
+      <c r="F99" s="0"/>
+      <c r="G99" s="0"/>
+      <c r="H99" s="0"/>
+      <c r="I99" s="0"/>
+      <c r="J99" s="0"/>
+      <c r="K99" s="0"/>
+      <c r="L99" s="0"/>
+      <c r="M99" s="0"/>
       <c r="N99" s="2"/>
       <c r="O99" s="2"/>
       <c r="P99" s="2"/>
@@ -3278,22 +3459,18 @@
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2"/>
-      <c r="B100" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C100" s="29"/>
-      <c r="D100" s="29"/>
-      <c r="E100" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F100" s="30"/>
-      <c r="G100" s="31"/>
-      <c r="H100" s="30"/>
-      <c r="I100" s="31"/>
-      <c r="J100" s="30"/>
-      <c r="K100" s="31"/>
-      <c r="L100" s="30"/>
-      <c r="M100" s="31"/>
+      <c r="B100" s="0"/>
+      <c r="C100" s="0"/>
+      <c r="D100" s="0"/>
+      <c r="E100" s="0"/>
+      <c r="F100" s="0"/>
+      <c r="G100" s="0"/>
+      <c r="H100" s="0"/>
+      <c r="I100" s="0"/>
+      <c r="J100" s="0"/>
+      <c r="K100" s="0"/>
+      <c r="L100" s="0"/>
+      <c r="M100" s="0"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
@@ -3313,18 +3490,18 @@
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
-      <c r="M101" s="2"/>
+      <c r="B101" s="0"/>
+      <c r="C101" s="0"/>
+      <c r="D101" s="0"/>
+      <c r="E101" s="0"/>
+      <c r="F101" s="0"/>
+      <c r="G101" s="0"/>
+      <c r="H101" s="0"/>
+      <c r="I101" s="0"/>
+      <c r="J101" s="0"/>
+      <c r="K101" s="0"/>
+      <c r="L101" s="0"/>
+      <c r="M101" s="0"/>
       <c r="N101" s="2"/>
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
@@ -3344,18 +3521,18 @@
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
-      <c r="M102" s="2"/>
+      <c r="B102" s="0"/>
+      <c r="C102" s="0"/>
+      <c r="D102" s="0"/>
+      <c r="E102" s="0"/>
+      <c r="F102" s="0"/>
+      <c r="G102" s="0"/>
+      <c r="H102" s="0"/>
+      <c r="I102" s="0"/>
+      <c r="J102" s="0"/>
+      <c r="K102" s="0"/>
+      <c r="L102" s="0"/>
+      <c r="M102" s="0"/>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
@@ -3375,18 +3552,18 @@
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-      <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
-      <c r="L103" s="2"/>
-      <c r="M103" s="2"/>
+      <c r="B103" s="0"/>
+      <c r="C103" s="0"/>
+      <c r="D103" s="0"/>
+      <c r="E103" s="0"/>
+      <c r="F103" s="0"/>
+      <c r="G103" s="0"/>
+      <c r="H103" s="0"/>
+      <c r="I103" s="0"/>
+      <c r="J103" s="0"/>
+      <c r="K103" s="0"/>
+      <c r="L103" s="0"/>
+      <c r="M103" s="0"/>
       <c r="N103" s="2"/>
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
@@ -3406,18 +3583,18 @@
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
-      <c r="M104" s="2"/>
+      <c r="B104" s="0"/>
+      <c r="C104" s="0"/>
+      <c r="D104" s="0"/>
+      <c r="E104" s="0"/>
+      <c r="F104" s="0"/>
+      <c r="G104" s="0"/>
+      <c r="H104" s="0"/>
+      <c r="I104" s="0"/>
+      <c r="J104" s="0"/>
+      <c r="K104" s="0"/>
+      <c r="L104" s="0"/>
+      <c r="M104" s="0"/>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
@@ -3437,18 +3614,18 @@
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="2"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
-      <c r="L105" s="2"/>
-      <c r="M105" s="2"/>
+      <c r="B105" s="0"/>
+      <c r="C105" s="0"/>
+      <c r="D105" s="0"/>
+      <c r="E105" s="0"/>
+      <c r="F105" s="0"/>
+      <c r="G105" s="0"/>
+      <c r="H105" s="0"/>
+      <c r="I105" s="0"/>
+      <c r="J105" s="0"/>
+      <c r="K105" s="0"/>
+      <c r="L105" s="0"/>
+      <c r="M105" s="0"/>
       <c r="N105" s="2"/>
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
@@ -3468,18 +3645,18 @@
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
-      <c r="M106" s="2"/>
+      <c r="B106" s="0"/>
+      <c r="C106" s="0"/>
+      <c r="D106" s="0"/>
+      <c r="E106" s="0"/>
+      <c r="F106" s="0"/>
+      <c r="G106" s="0"/>
+      <c r="H106" s="0"/>
+      <c r="I106" s="0"/>
+      <c r="J106" s="0"/>
+      <c r="K106" s="0"/>
+      <c r="L106" s="0"/>
+      <c r="M106" s="0"/>
       <c r="N106" s="2"/>
       <c r="O106" s="2"/>
       <c r="P106" s="2"/>
@@ -3499,18 +3676,18 @@
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-      <c r="L107" s="2"/>
-      <c r="M107" s="2"/>
+      <c r="B107" s="0"/>
+      <c r="C107" s="0"/>
+      <c r="D107" s="0"/>
+      <c r="E107" s="0"/>
+      <c r="F107" s="0"/>
+      <c r="G107" s="0"/>
+      <c r="H107" s="0"/>
+      <c r="I107" s="0"/>
+      <c r="J107" s="0"/>
+      <c r="K107" s="0"/>
+      <c r="L107" s="0"/>
+      <c r="M107" s="0"/>
       <c r="N107" s="2"/>
       <c r="O107" s="2"/>
       <c r="P107" s="2"/>
@@ -3530,18 +3707,18 @@
     </row>
     <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
-      <c r="L108" s="2"/>
-      <c r="M108" s="2"/>
+      <c r="B108" s="0"/>
+      <c r="C108" s="0"/>
+      <c r="D108" s="0"/>
+      <c r="E108" s="0"/>
+      <c r="F108" s="0"/>
+      <c r="G108" s="0"/>
+      <c r="H108" s="0"/>
+      <c r="I108" s="0"/>
+      <c r="J108" s="0"/>
+      <c r="K108" s="0"/>
+      <c r="L108" s="0"/>
+      <c r="M108" s="0"/>
       <c r="N108" s="2"/>
       <c r="O108" s="2"/>
       <c r="P108" s="2"/>

</xml_diff>